<commit_message>
- My Second Commit
</commit_message>
<xml_diff>
--- a/orders_export1265-6-2.xlsx
+++ b/orders_export1265-6-2.xlsx
@@ -8712,7 +8712,7 @@
     <t>LT112191375CN</t>
   </si>
   <si>
-    <t>version 4.0</t>
+    <t>version 5.0</t>
   </si>
 </sst>
 </file>
@@ -70046,7 +70046,7 @@
   <dimension ref="A1:J279"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>

</xml_diff>